<commit_message>
fix: corrigindo média do grafico
</commit_message>
<xml_diff>
--- a/trezentosteste999.xlsx
+++ b/trezentosteste999.xlsx
@@ -327,7 +327,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,8 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -356,8 +355,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -366,8 +364,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -376,8 +373,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -386,8 +382,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -396,8 +391,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -406,7 +400,6 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
         <v>11</v>
       </c>
       <c r="D8" s="2"/>
@@ -416,8 +409,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -426,8 +418,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -436,8 +427,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -446,8 +436,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -456,8 +445,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -466,8 +454,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -476,8 +463,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -486,8 +472,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -496,8 +481,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -506,8 +490,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -516,8 +499,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -526,8 +508,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -536,8 +517,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -546,8 +526,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="n">
-        <f aca="false">RANDBETWEEN(0,14)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
fix: adicionando aleatoriedade a planilha do excel novamente
</commit_message>
<xml_diff>
--- a/trezentosteste999.xlsx
+++ b/trezentosteste999.xlsx
@@ -327,7 +327,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B22"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,7 +346,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>9</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -355,7 +356,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>3</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -364,7 +366,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>1</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -373,7 +376,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>4</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -382,7 +386,8 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>14</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -391,7 +396,8 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>0</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -400,7 +406,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>0</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -409,7 +416,8 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>8</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -418,7 +426,8 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>6</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -427,7 +436,8 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>9</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -436,7 +446,8 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>5</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -445,6 +456,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
         <v>11</v>
       </c>
       <c r="D13" s="2"/>
@@ -454,7 +466,8 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>14</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -463,7 +476,8 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>14</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -472,7 +486,8 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>8</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -481,7 +496,8 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>12</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -490,7 +506,8 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>5</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -499,7 +516,8 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>9</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -508,7 +526,8 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>8</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -517,7 +536,8 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>14</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -526,7 +546,8 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>11</v>
+        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
+        <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
adicionando a medalha ao grafico base
</commit_message>
<xml_diff>
--- a/trezentosteste999.xlsx
+++ b/trezentosteste999.xlsx
@@ -324,10 +324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,7 +347,7 @@
       </c>
       <c r="B2" s="2" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B20" s="2" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B21" s="2" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -547,11 +547,19 @@
       </c>
       <c r="B22" s="2" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>